<commit_message>
add a sheet of sensors data
</commit_message>
<xml_diff>
--- a/cyber_traits_project.xlsx
+++ b/cyber_traits_project.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yafit Shneor\GitHub\cyberTraits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onaki\Downloads\cyberTraits-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4C725A-74F1-4CE8-866F-66425B3E1C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70975497-3168-4423-B490-87A7658AB711}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1E004A04-5E3F-4E0A-BD1B-1F5248A47DD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1E004A04-5E3F-4E0A-BD1B-1F5248A47DD5}"/>
   </bookViews>
   <sheets>
     <sheet name="data from the beiwe app" sheetId="1" r:id="rId1"/>
-    <sheet name="&quot;מאמר &quot;התחלת המסע " sheetId="4" r:id="rId2"/>
+    <sheet name="sensors data" sheetId="5" r:id="rId2"/>
+    <sheet name="&quot;מאמר &quot;התחלת המסע " sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="202">
   <si>
     <t>Column1</t>
   </si>
@@ -305,7 +312,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -345,7 +352,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -419,7 +426,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -428,8 +435,8 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">MAD = 1/n ∑ | ri - r' |
-מחשבים את זה לכל שעה ביום, ואת עושים ממוצע של של כל שעה בימים הנבדקים.
+      <t xml:space="preserve">סטיית תקן:
+מחשבים סטיית תקן של שלושת ערכי המיקום לפי בוקר, ערב ולילה, ועליהם עושים ממוצע.
 </t>
     </r>
     <r>
@@ -437,27 +444,17 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>סה"כ 24 נתונים</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">סטיית תקן:
-מחשבים סטיית תקן של שלושת ערכי המיקום לפי בוקר, ערב ולילה, ועליהם עושים ממוצע.
+      <t>סה"כ 9 נתונים.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">מחשבים את מספר הMACים השונים שהמשתמש נמצא בקרבתם בבוקר, ערב ולילה.
+עליהם עושים ממוצע וסטיית תקן על כל הימים הנבדקים- בוקר, ערב ולילה.
 </t>
     </r>
     <r>
@@ -465,38 +462,20 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>סה"כ 9 נתונים.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">מחשבים את מספר הMACים השונים שהמשתמש נמצא בקרבתם בבוקר, ערב ולילה.
-עליהם עושים ממוצע וסטיית תקן על כל הימים הנבדקים- בוקר, ערב ולילה.
-</t>
-    </r>
+      <t>סה"כ 6 נתונים.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>סה"כ 6 נתונים.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -506,7 +485,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -525,7 +504,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -535,7 +514,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -572,16 +551,442 @@
 הם בעצם התמקדו בלמוצא 3 דברים: דיכאון, רגולריות ומגוון.</t>
     </r>
   </si>
+  <si>
+    <t>sensor</t>
+  </si>
+  <si>
+    <t>file name</t>
+  </si>
+  <si>
+    <t>column 1</t>
+  </si>
+  <si>
+    <t>column 2</t>
+  </si>
+  <si>
+    <t>column 3</t>
+  </si>
+  <si>
+    <t>column 4</t>
+  </si>
+  <si>
+    <t>column 5</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd hh_mm_ss</t>
+  </si>
+  <si>
+    <t>folder name</t>
+  </si>
+  <si>
+    <t>power states</t>
+  </si>
+  <si>
+    <t>power_state</t>
+  </si>
+  <si>
+    <t>wifi</t>
+  </si>
+  <si>
+    <t>survey answers</t>
+  </si>
+  <si>
+    <t>survey_answers</t>
+  </si>
+  <si>
+    <t>survey timings</t>
+  </si>
+  <si>
+    <t>survey_timings</t>
+  </si>
+  <si>
+    <t>relevant for research</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>UTC time</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>column 6</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MAD = 1/n ∑ | ri - r' |
+מחשבים את זה לכל שעה ביום, ואז עושים ממוצע של של כל שעה בימים הנבדקים.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>סה"כ 24 נתונים</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>explanation column 1</t>
+  </si>
+  <si>
+    <t>explanation column 2</t>
+  </si>
+  <si>
+    <t>explanation column 3</t>
+  </si>
+  <si>
+    <t>explanation column 4</t>
+  </si>
+  <si>
+    <t>explanation column 5</t>
+  </si>
+  <si>
+    <t>explanation column 6</t>
+  </si>
+  <si>
+    <t>תאוצה על ציר ה-X</t>
+  </si>
+  <si>
+    <t>תאוצה על ציר ה-Y</t>
+  </si>
+  <si>
+    <t>תאוצה על ציר ה-Z</t>
+  </si>
+  <si>
+    <t>אנו מחשבות עבור כל שעה את ה-MAD שלה. 
+בכל שעה אנו בודקים כל שניה. אם יש שניה שבה אין לנו מידע על התאוצה, אנו נסמן את זמן זה ב-0,0,0, כיון שלא היתה תאוצה בזמן זה. לוקחים את כל נתוני התאוצה על שלושלת המימדים, ומחשבים MAD(מתואר בעמוד המאמר), כאשר N=60*60</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">רצף של ספרות המרכיבות את התאריך והשעה בו התרחש האירוע.
+מוצג באופן עקבי עולה לצורך השוואה.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not in use</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">yyyy-MM-ddThh:mm:ss.mmm
+(2019-11-07T13:24:39.313)
+</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>1. ישנם מכשירים שלא דוגמים את מד התאוצה כאשר המסך מכובה.
+2. ישנם מכשירים שמנטרלים לגמרי את דגימות התאוצה.
+3. נתוני התאוצה יתקבלו במרחב [20,20-] אך ישנם מכשירים שהנתונים בהם יהיו במרחב [10,10-].</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>yyyy-MM-ddThh:mm:ss.mmm
+(2019-11-07T13:24:39.313)</t>
+  </si>
+  <si>
+    <t>מצבי מסך המכשיר:
+1. Device Idle (Doze) state change signal received; device in idle state.
+כאשר המסך מכובה, התאוצה מינימלית ולא מוטען. סוג של מצב שינה. יוצא ממצב זה, כאשר צריך לעשות משימות ברקע.
+2. Device Idle (Doze) state change signal received; device not in idle state.
+אין לזה מידע מפורט בANDROID.
+3. Screen turned on
+כאשר המסך נדלק.
+4. Screen turned off
+כאשר המסך נכבה.</t>
+  </si>
+  <si>
+    <t>__</t>
+  </si>
+  <si>
+    <t>1. סוכמים את משך הזמן בו המכשיר היה דלוק, ז"א מאז שנדלק עד שנכבה. סוכמים זאת עבור כל חלק זמן ביום- יום, ערב ולילה. עבור כל חלק ביום אנו מחשבים ממוצע וסטיית תקן.
+2. סופרים כמה פעמים המכשיר הודלק. סופרים זאת עבור כל חלק ביום- יום, ערב ולילה. עבור כל חלק ביום מחשבים ממוצע וסטיית תקן.</t>
+  </si>
+  <si>
+    <t>אנו לא מתייחסים למצבים 1, 2.</t>
+  </si>
+  <si>
+    <t>Not in use</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>altitude</t>
+  </si>
+  <si>
+    <t>קו רוחב- מציין עד כמה נקודה על פני כדור הארץ נמצאת מדרום או מצפון לקו המשוה.</t>
+  </si>
+  <si>
+    <t>קו אורך- מציין עד כמה נקודה על פני כדור הארץ נמצאת ממזרח או ממערב לקו גריניץ'.</t>
+  </si>
+  <si>
+    <t>כל 5 דקות מחשבים את המרחק שעברנו. אם אין מידע על הזמן הספיצפי הזה, לוקחים את המידע על המיקום האחרון שנקלט (לא נרשם שינוי במיקום -&gt; נמצא באותו מקום).
+סוכמים את המרחקים שעברנו עבור כל חלק ביום- יום, ערב ולילה. ועל זה מחשבים ממוצע וסטיית תקן.</t>
+  </si>
+  <si>
+    <t>חישוב במרחק, נעשה ע"י פונקציה קיימת המחשבת מרחקים בין נקודות על הגלובוס.
+פונקציה זו מחשבת מרחקים אוויריים.</t>
+  </si>
+  <si>
+    <t>hashed MAC</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>RSSI</t>
+  </si>
+  <si>
+    <t>מספר ה-MAC של מכשיר ה-WIFI שנמצא בסביבת המכשיר.
+ה-MAC מגיע בצורה מוצפנת.</t>
+  </si>
+  <si>
+    <t>תמיד יהיה 2.4GHZ או 5GHZ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סופרים עבור כל חלק ביום, כמה WIFI שונים היו בסביבת במכשיר.
+על זה מחשבים ממוצע וסטיית תקן. </t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>bluetooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סופרים עבור כל חלק ביום, כמה מכשירים שונים היו בסביבת במכשיר.
+על זה מחשבים ממוצע וסטיית תקן. </t>
+  </si>
+  <si>
+    <t>שם המשתמש של המכשיר באפליקציה</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>מספר ה-MAC המוצפן של המכשיר</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>מספר הטלפון המוצפן של המכשיר</t>
+  </si>
+  <si>
+    <t>device_id</t>
+  </si>
+  <si>
+    <t>device_os</t>
+  </si>
+  <si>
+    <t>column 7</t>
+  </si>
+  <si>
+    <t>column 8</t>
+  </si>
+  <si>
+    <t>column 9</t>
+  </si>
+  <si>
+    <t>column 10</t>
+  </si>
+  <si>
+    <t>column 11</t>
+  </si>
+  <si>
+    <t>explanation column 7</t>
+  </si>
+  <si>
+    <t>explanation column 8</t>
+  </si>
+  <si>
+    <t>explanation column 9</t>
+  </si>
+  <si>
+    <t>explanation column 10</t>
+  </si>
+  <si>
+    <t>explanation column 11</t>
+  </si>
+  <si>
+    <t>explanation column 14</t>
+  </si>
+  <si>
+    <t>explanation column 13</t>
+  </si>
+  <si>
+    <t>explanation column 12</t>
+  </si>
+  <si>
+    <t>column 14</t>
+  </si>
+  <si>
+    <t>column 13</t>
+  </si>
+  <si>
+    <t>column 12</t>
+  </si>
+  <si>
+    <t>מערכת הפעלה של המכשיר לדוג אנדרואיד</t>
+  </si>
+  <si>
+    <t>os_version</t>
+  </si>
+  <si>
+    <t>גרסת מערכת הפעלה</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>hardware_id</t>
+  </si>
+  <si>
+    <t>זיהוי חומרה</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>גרסת המכשיר</t>
+  </si>
+  <si>
+    <t>beiwe_version</t>
+  </si>
+  <si>
+    <t>גרסת האפליקציה</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>זיהוי המכשיר</t>
+  </si>
+  <si>
+    <t>שם חברת הפלאפון. 
+לדוג נוקייה.</t>
+  </si>
+  <si>
+    <t>X
+we are not using the app surveys</t>
+  </si>
+  <si>
+    <t>X 
+we are not using the app surveys</t>
+  </si>
+  <si>
+    <t>the data we are taking</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">אינדיקציה לחוזק האות שהתקבל. מתקבל ב-DBm.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not in use</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">קו גובה- מציין גובה המיקום על פני הים.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not in use</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">דיוק- עד כמה הנתונים מדוייקים, במטרים.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not in use</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -601,7 +1006,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -609,20 +1014,46 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -630,11 +1061,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -668,6 +1114,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,7 +1366,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1182,19 +1664,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB7DC93-3FDB-4E1D-9AC1-2E3E85A60D4E}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="D1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.09765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.69921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="56.296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="56.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="6" width="46.69921875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.09765625" style="1"/>
+    <col min="6" max="6" width="46.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1220,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1237,10 +1719,10 @@
         <v>37</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1257,10 +1739,10 @@
         <v>39</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1277,7 +1759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="110.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1294,10 +1776,10 @@
         <v>41</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="110.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1314,10 +1796,10 @@
         <v>44</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1334,7 +1816,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1354,7 +1836,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1371,7 +1853,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="69" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1385,7 +1867,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="69" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1402,7 +1884,7 @@
         <v>88</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1416,23 +1898,832 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE76D2F-DA2A-4FCB-9788-EADCB0275E20}">
+  <dimension ref="A1:AI9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="13" style="13" customWidth="1"/>
+    <col min="10" max="10" width="20" style="13" customWidth="1"/>
+    <col min="11" max="11" width="12" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" style="13" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="13" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="13" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" style="13" customWidth="1"/>
+    <col min="16" max="23" width="20" style="13" customWidth="1"/>
+    <col min="24" max="24" width="22.5703125" style="13" customWidth="1"/>
+    <col min="25" max="25" width="20" style="13" customWidth="1"/>
+    <col min="26" max="26" width="22.28515625" style="13" customWidth="1"/>
+    <col min="27" max="27" width="20" style="13" customWidth="1"/>
+    <col min="28" max="28" width="24.5703125" style="13" customWidth="1"/>
+    <col min="29" max="29" width="20" style="13" customWidth="1"/>
+    <col min="30" max="30" width="21.28515625" style="13" customWidth="1"/>
+    <col min="31" max="31" width="20" style="13" customWidth="1"/>
+    <col min="32" max="32" width="21.85546875" style="13" customWidth="1"/>
+    <col min="33" max="33" width="21.7109375" style="18" customWidth="1"/>
+    <col min="34" max="36" width="19.28515625" style="13" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" s="23" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="W1" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA1" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB1" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="AC1" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE1" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="AF1" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="AG1" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="AH1" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="AI1" s="20"/>
+    </row>
+    <row r="2" spans="1:35" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="315" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG3" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="195" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG4" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH4" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="R5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="V5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="W5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="X5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG5" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="T6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="V6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="W6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="X6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG6" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="W7" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="X7" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y7" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z7" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA7" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC7" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD7" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE7" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF7" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762BC438-58B3-4923-B652-B49F40252BF1}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:J22"/>
+    <sheetView rightToLeft="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.09765625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="29" style="5" customWidth="1"/>
-    <col min="3" max="3" width="49.3984375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.59765625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="21" style="5" customWidth="1"/>
     <col min="6" max="6" width="26" style="6" customWidth="1"/>
     <col min="7" max="9" width="9" style="5"/>
-    <col min="10" max="10" width="9.3984375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="5" customWidth="1"/>
     <col min="11" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
@@ -1468,7 +2759,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
@@ -1482,10 +2773,10 @@
         <v>66</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="110.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1525,7 +2816,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>80</v>
       </c>
@@ -1545,7 +2836,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>80</v>
       </c>
@@ -1572,7 +2863,7 @@
     </row>
     <row r="22" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>

</xml_diff>